<commit_message>
UWP (re)Sizing is working.
</commit_message>
<xml_diff>
--- a/UWP_Sizes.xlsx
+++ b/UWP_Sizes.xlsx
@@ -110,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -122,6 +122,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,28 +580,29 @@
       </c>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
       <c r="B22" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C22" s="5">
-        <v>533.33331298828102</v>
+        <v>500</v>
       </c>
       <c r="D22" s="5">
-        <v>-139.999989282607</v>
+        <v>-115</v>
       </c>
       <c r="E22" s="5">
-        <v>0.6</v>
+        <v>0.67895174917131795</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="5">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="5">
-        <v>568.888916015625</v>
+        <v>533.33331298828102</v>
       </c>
       <c r="D23" s="5">
-        <v>-75</v>
+        <v>-139.999989282607</v>
       </c>
       <c r="E23" s="5">
         <v>0.6</v>
@@ -608,27 +610,27 @@
     </row>
     <row r="24" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="C24" s="5">
-        <v>640</v>
+        <v>568.888916015625</v>
       </c>
       <c r="D24" s="5">
-        <v>-37.697788104944003</v>
+        <v>-75</v>
       </c>
       <c r="E24" s="5">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5">
-        <v>5.2</v>
+        <v>5</v>
       </c>
       <c r="C25" s="5">
         <v>640</v>
       </c>
       <c r="D25" s="5">
-        <v>-59.770918468501101</v>
+        <v>-37.697788104944003</v>
       </c>
       <c r="E25" s="5">
         <v>0.75</v>
@@ -636,15 +638,29 @@
     </row>
     <row r="26" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="C26" s="5">
+        <v>640</v>
+      </c>
+      <c r="D26" s="5">
+        <v>-59.770918468501101</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="5">
         <v>6</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C27" s="5">
         <v>768</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D27" s="5">
         <v>-9.4622469738706005</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E27" s="5">
         <v>0.9</v>
       </c>
     </row>

</xml_diff>